<commit_message>
Changed male sex column name from 'H' to 'M' (just makes more sense)
</commit_message>
<xml_diff>
--- a/Datasheet1-sex&age.xlsx
+++ b/Datasheet1-sex&age.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Hugo/Documents/GitHub/Cancer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBB12B2D-145E-F941-9A4A-DAD9B51139A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F60648F-8901-E442-AE08-70B14C6875B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25660" yWindow="500" windowWidth="20120" windowHeight="10340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16180" yWindow="500" windowWidth="22220" windowHeight="11980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,13 +38,13 @@
     <t>F</t>
   </si>
   <si>
-    <t>H</t>
+    <t>F_canc</t>
   </si>
   <si>
-    <t>H_canc</t>
+    <t>M</t>
   </si>
   <si>
-    <t>F_canc</t>
+    <t>M_canc</t>
   </si>
 </sst>
 </file>
@@ -171,8 +171,8 @@
   <autoFilter ref="A1:D90" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="F"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="H"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="H_canc"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="M"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="M_canc"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="F_canc"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -469,8 +469,8 @@
   </sheetPr>
   <dimension ref="A1:H90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -487,13 +487,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>